<commit_message>
v0.1 add + pagedown
</commit_message>
<xml_diff>
--- a/2018-03月份绩效填写用表.xlsx
+++ b/2018-03月份绩效填写用表.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nzy-6\MyPython\AutoAchievements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutoAchievements\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E133F5AB-4C54-4125-B885-95780B1C1574}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24615" windowHeight="8040" xr2:uid="{F4240D48-ED6F-4F17-9F36-30A08820576D}"/>
   </bookViews>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t xml:space="preserve">完成功能点等于 100%，不扣分； 完成功能点每低 于%1，对应分数 扣除1分。 </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -54,23 +55,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0.25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>移动端后台管理1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>移动端后台管理2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>移动端后台管理3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>移动端后台管理4</t>
+    <t>0.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>后台系统优化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>财务报表优化二期</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -438,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D381E064-40DB-4608-873D-71FE37504F37}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="A4" sqref="A4:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -473,7 +470,7 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -488,45 +485,15 @@
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>